<commit_message>
Trying to get HUCs for each watershed
</commit_message>
<xml_diff>
--- a/FireMeta_Rproj/inputs/Studies_Summary/Fire_name_Lat_Long.xlsx
+++ b/FireMeta_Rproj/inputs/Studies_Summary/Fire_name_Lat_Long.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cava304/GitHub/rc_sfa-rc-3-wenas-meta/FireMeta_Rproj/inputs/Studies_Summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA2E940-EFEE-EC41-BE41-F14841817A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD3FAA7-7B48-E44D-9513-25B89F7D683F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" activeTab="1" xr2:uid="{8C258C6F-044A-E849-9C14-F26FA5F5AA92}"/>
+    <workbookView xWindow="35620" yWindow="700" windowWidth="30240" windowHeight="17260" xr2:uid="{8C258C6F-044A-E849-9C14-F26FA5F5AA92}"/>
   </bookViews>
   <sheets>
     <sheet name="Temporal Normalization Studies" sheetId="1" r:id="rId1"/>
-    <sheet name="Fires we don’t have yet" sheetId="2" r:id="rId2"/>
+    <sheet name="Katie_code_format" sheetId="3" r:id="rId2"/>
+    <sheet name="Fires we don’t have yet" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="128">
   <si>
     <t>Study</t>
   </si>
@@ -459,6 +460,15 @@
   </si>
   <si>
     <t xml:space="preserve">44.578525	</t>
+  </si>
+  <si>
+    <t>site</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
   </si>
 </sst>
 </file>
@@ -567,7 +577,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -586,6 +596,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -599,7 +615,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -622,19 +638,14 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -951,9 +962,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE608700-CF3C-DE4E-8B7D-38FBD72A91DD}">
   <dimension ref="A1:K81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D40" sqref="D40:E40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" activeCellId="1" sqref="B22:B23 D22:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1105,10 +1116,10 @@
         <v>32</v>
       </c>
       <c r="D7">
-        <v>34.477563000000004</v>
+        <v>34.484966</v>
       </c>
       <c r="E7">
-        <v>-120.21596599999999</v>
+        <v>-120.22992600000001</v>
       </c>
       <c r="F7">
         <v>52.16</v>
@@ -2898,19 +2909,884 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F70F01-B0DC-C845-8599-5B62D652F3A7}">
+  <dimension ref="A1:I46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="7">
+        <v>40.133513999999998</v>
+      </c>
+      <c r="I1" s="7">
+        <v>-111.771241</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2">
+        <v>48.814951999999998</v>
+      </c>
+      <c r="C2">
+        <v>-113.983313</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="7">
+        <v>40.180647</v>
+      </c>
+      <c r="I2" s="7">
+        <v>-111.67166400000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3">
+        <v>48.936976000000001</v>
+      </c>
+      <c r="C3">
+        <v>-114.079685</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3">
+        <v>40.191034999999999</v>
+      </c>
+      <c r="I3">
+        <v>-111.65993899999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4">
+        <v>48.866349</v>
+      </c>
+      <c r="C4">
+        <v>-114.02640599999999</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4">
+        <v>40.158754000000002</v>
+      </c>
+      <c r="I4">
+        <v>-111.59730999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5">
+        <v>38.883760000000002</v>
+      </c>
+      <c r="C5">
+        <v>-119.978005</v>
+      </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5">
+        <v>40.200989</v>
+      </c>
+      <c r="I5">
+        <v>-111.659265</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6">
+        <v>38.898688999999997</v>
+      </c>
+      <c r="C6">
+        <v>-119.948785</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6">
+        <v>40.192393000000003</v>
+      </c>
+      <c r="I6">
+        <v>-111.652799</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7">
+        <v>38.958700999999998</v>
+      </c>
+      <c r="C7">
+        <v>-120.920501</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="7">
+        <v>39.987803999999997</v>
+      </c>
+      <c r="I7" s="7">
+        <v>-111.72989099999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8">
+        <v>39.000053000000001</v>
+      </c>
+      <c r="C8">
+        <v>-120.93990700000001</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="29">
+        <v>40.234889000000003</v>
+      </c>
+      <c r="I8" s="29">
+        <v>-111.724869</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9">
+        <v>39.906348000000001</v>
+      </c>
+      <c r="C9">
+        <v>-105.37748499999999</v>
+      </c>
+      <c r="G9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9">
+        <v>40.071703999999997</v>
+      </c>
+      <c r="I9">
+        <v>-111.57715</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10">
+        <v>48.422220000000003</v>
+      </c>
+      <c r="C10">
+        <v>-113.70055549999999</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="29">
+        <v>40.071703999999997</v>
+      </c>
+      <c r="I10" s="29">
+        <v>-111.57715</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11">
+        <v>48.54888888</v>
+      </c>
+      <c r="C11">
+        <v>-113.9858333</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11">
+        <v>44.515999999999998</v>
+      </c>
+      <c r="I11">
+        <v>-110.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12">
+        <v>48.635277780000003</v>
+      </c>
+      <c r="C12">
+        <v>-113.86694439999999</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12">
+        <v>44.555</v>
+      </c>
+      <c r="I12">
+        <v>-110.069</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13">
+        <v>48.635277780000003</v>
+      </c>
+      <c r="C13">
+        <v>-113.86694439999999</v>
+      </c>
+      <c r="G13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13">
+        <v>48.81409</v>
+      </c>
+      <c r="I13">
+        <v>-114.39971</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="5">
+        <v>40.039045999999999</v>
+      </c>
+      <c r="C14" s="9">
+        <v>-105.393878</v>
+      </c>
+      <c r="G14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14">
+        <v>48.793787000000002</v>
+      </c>
+      <c r="I14">
+        <v>-114.49179100000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="5">
+        <v>40.041668000000001</v>
+      </c>
+      <c r="C15" s="9">
+        <v>-105.364823</v>
+      </c>
+      <c r="G15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15">
+        <v>48.802771999999997</v>
+      </c>
+      <c r="I15">
+        <v>-114.32894</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="5">
+        <v>40.015500000000003</v>
+      </c>
+      <c r="C16" s="9">
+        <v>-105.324566</v>
+      </c>
+      <c r="G16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16">
+        <v>48.688412999999997</v>
+      </c>
+      <c r="I16">
+        <v>-114.19973899999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="5">
+        <v>40.036102999999997</v>
+      </c>
+      <c r="C17" s="9">
+        <v>-105.43910099999999</v>
+      </c>
+      <c r="G17" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17">
+        <v>48.902925000000003</v>
+      </c>
+      <c r="I17">
+        <v>-114.183566</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18">
+        <v>40.037790999999999</v>
+      </c>
+      <c r="C18" s="10">
+        <v>-105.42124699999999</v>
+      </c>
+      <c r="G18" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18">
+        <v>48.814951999999998</v>
+      </c>
+      <c r="I18">
+        <v>-113.983313</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="5">
+        <v>40.039045999999999</v>
+      </c>
+      <c r="C19" s="9">
+        <v>-105.393878</v>
+      </c>
+      <c r="G19" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19">
+        <v>48.936976000000001</v>
+      </c>
+      <c r="I19">
+        <v>-114.079685</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="5">
+        <v>40.041668000000001</v>
+      </c>
+      <c r="C20" s="9">
+        <v>-105.364823</v>
+      </c>
+      <c r="G20" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20">
+        <v>48.866349</v>
+      </c>
+      <c r="I20">
+        <v>-114.02640599999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="5">
+        <v>40.015500000000003</v>
+      </c>
+      <c r="C21" s="9">
+        <v>-105.324566</v>
+      </c>
+      <c r="G21" t="s">
+        <v>60</v>
+      </c>
+      <c r="H21">
+        <v>38.883760000000002</v>
+      </c>
+      <c r="I21">
+        <v>-119.978005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="5">
+        <v>40.036102999999997</v>
+      </c>
+      <c r="C22" s="9">
+        <v>-105.43910099999999</v>
+      </c>
+      <c r="G22" t="s">
+        <v>87</v>
+      </c>
+      <c r="H22">
+        <v>38.898688999999997</v>
+      </c>
+      <c r="I22">
+        <v>-119.948785</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23">
+        <v>34.937945999999997</v>
+      </c>
+      <c r="C23">
+        <v>-83.093596000000005</v>
+      </c>
+      <c r="G23" t="s">
+        <v>61</v>
+      </c>
+      <c r="H23">
+        <v>38.958700999999998</v>
+      </c>
+      <c r="I23">
+        <v>-120.920501</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24">
+        <v>34.920959000000003</v>
+      </c>
+      <c r="C24">
+        <v>-83.092200000000005</v>
+      </c>
+      <c r="G24" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24">
+        <v>39.000053000000001</v>
+      </c>
+      <c r="I24">
+        <v>-120.93990700000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25">
+        <v>38.868000000000002</v>
+      </c>
+      <c r="C25">
+        <v>-120.062</v>
+      </c>
+      <c r="G25" t="s">
+        <v>63</v>
+      </c>
+      <c r="H25">
+        <v>39.906348000000001</v>
+      </c>
+      <c r="I25">
+        <v>-105.37748499999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26">
+        <v>38.880000000000003</v>
+      </c>
+      <c r="C26">
+        <v>-120.041</v>
+      </c>
+      <c r="G26" t="s">
+        <v>64</v>
+      </c>
+      <c r="H26">
+        <v>48.422220000000003</v>
+      </c>
+      <c r="I26">
+        <v>-113.70055549999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27">
+        <v>38.878999999999998</v>
+      </c>
+      <c r="C27">
+        <v>-120.03</v>
+      </c>
+      <c r="G27" t="s">
+        <v>65</v>
+      </c>
+      <c r="H27">
+        <v>48.54888888</v>
+      </c>
+      <c r="I27">
+        <v>-113.9858333</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28">
+        <v>38.872999999999998</v>
+      </c>
+      <c r="C28">
+        <v>-120.01300000000001</v>
+      </c>
+      <c r="G28" t="s">
+        <v>66</v>
+      </c>
+      <c r="H28">
+        <v>48.635277780000003</v>
+      </c>
+      <c r="I28">
+        <v>-113.86694439999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="G29" t="s">
+        <v>67</v>
+      </c>
+      <c r="H29">
+        <v>48.635277780000003</v>
+      </c>
+      <c r="I29">
+        <v>-113.86694439999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="G30" t="s">
+        <v>68</v>
+      </c>
+      <c r="H30" s="5">
+        <v>40.039045999999999</v>
+      </c>
+      <c r="I30" s="9">
+        <v>-105.393878</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31">
+        <v>38.451371999999999</v>
+      </c>
+      <c r="C31">
+        <v>122.056381</v>
+      </c>
+      <c r="G31" t="s">
+        <v>69</v>
+      </c>
+      <c r="H31" s="5">
+        <v>40.041668000000001</v>
+      </c>
+      <c r="I31" s="9">
+        <v>-105.364823</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" s="6">
+        <v>38.923563999999999</v>
+      </c>
+      <c r="C32" s="6">
+        <v>122.32647799999999</v>
+      </c>
+      <c r="G32" t="s">
+        <v>70</v>
+      </c>
+      <c r="H32" s="5">
+        <v>40.015500000000003</v>
+      </c>
+      <c r="I32" s="9">
+        <v>-105.324566</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33">
+        <v>38.512031</v>
+      </c>
+      <c r="C33">
+        <v>122.097228</v>
+      </c>
+      <c r="G33" t="s">
+        <v>71</v>
+      </c>
+      <c r="H33" s="5">
+        <v>40.036102999999997</v>
+      </c>
+      <c r="I33" s="9">
+        <v>-105.43910099999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34">
+        <v>40.728676</v>
+      </c>
+      <c r="C34">
+        <v>-105.844109</v>
+      </c>
+      <c r="G34" t="s">
+        <v>72</v>
+      </c>
+      <c r="H34">
+        <v>40.037790999999999</v>
+      </c>
+      <c r="I34" s="10">
+        <v>-105.42124699999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35">
+        <v>40.709603999999999</v>
+      </c>
+      <c r="C35">
+        <v>-105.233305</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H35">
+        <v>34.937945999999997</v>
+      </c>
+      <c r="I35">
+        <v>-83.093596000000005</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36">
+        <v>40.701225999999998</v>
+      </c>
+      <c r="C36">
+        <v>-105.757445</v>
+      </c>
+      <c r="G36" t="s">
+        <v>73</v>
+      </c>
+      <c r="H36">
+        <v>34.920959000000003</v>
+      </c>
+      <c r="I36">
+        <v>-83.092200000000005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37">
+        <v>40.728676</v>
+      </c>
+      <c r="C37">
+        <v>-105.844109</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H37">
+        <v>38.868000000000002</v>
+      </c>
+      <c r="I37">
+        <v>-120.062</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38">
+        <v>40.709603999999999</v>
+      </c>
+      <c r="C38">
+        <v>-105.233305</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H38">
+        <v>38.880000000000003</v>
+      </c>
+      <c r="I38">
+        <v>-120.041</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39">
+        <v>40.701225999999998</v>
+      </c>
+      <c r="C39">
+        <v>-105.757445</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H39">
+        <v>38.878999999999998</v>
+      </c>
+      <c r="I39">
+        <v>-120.03</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G40" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H40">
+        <v>38.872999999999998</v>
+      </c>
+      <c r="I40">
+        <v>-120.01300000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G41" t="s">
+        <v>81</v>
+      </c>
+      <c r="H41">
+        <v>38.451371999999999</v>
+      </c>
+      <c r="I41">
+        <v>-122.056381</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G42" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H42" s="6">
+        <v>38.923563999999999</v>
+      </c>
+      <c r="I42" s="6">
+        <v>-122.32647799999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G43" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H43">
+        <v>38.512031</v>
+      </c>
+      <c r="I43">
+        <v>-122.097228</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G44" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H44">
+        <v>40.728676</v>
+      </c>
+      <c r="I44">
+        <v>-105.844109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G45" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H45">
+        <v>40.709603999999999</v>
+      </c>
+      <c r="I45">
+        <v>-105.233305</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G46" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H46">
+        <v>40.701225999999998</v>
+      </c>
+      <c r="I46">
+        <v>-105.757445</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C17DF85F-2C1F-F649-BAF1-80C86400E080}">
   <dimension ref="A1:L78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.1640625" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.83203125" style="22"/>
-    <col min="5" max="5" width="38.1640625" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.83203125" style="22"/>
+    <col min="1" max="1" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="38.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2924,9 +3800,9 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -2965,7 +3841,7 @@
       <c r="A5" t="s">
         <v>108</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B5" s="22">
         <v>34.460483000000004</v>
       </c>
       <c r="C5" t="s">
@@ -2976,13 +3852,13 @@
       <c r="A6" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6">
         <v>36.095348999999999</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6">
         <v>-82.265000000000001</v>
       </c>
-      <c r="E6" s="26"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -3038,11 +3914,11 @@
       <c r="C11">
         <v>-116.1031</v>
       </c>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="22" t="s">
+      <c r="A12" t="s">
         <v>5</v>
       </c>
       <c r="B12">
@@ -3108,122 +3984,122 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="26"/>
+      <c r="A20" s="23"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="26"/>
+      <c r="A21" s="23"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="K22" s="9"/>
       <c r="L22" s="5"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="26"/>
-      <c r="E24" s="26"/>
+      <c r="A24" s="23"/>
+      <c r="E24" s="23"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="26"/>
+      <c r="A25" s="23"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="26"/>
+      <c r="A26" s="23"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E32" s="26"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
     </row>
     <row r="46" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E46" s="26"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="28"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="24"/>
     </row>
     <row r="52" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E52" s="30"/>
+      <c r="E52" s="26"/>
     </row>
     <row r="53" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E53" s="27"/>
-      <c r="F53" s="27"/>
-      <c r="G53" s="31"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="9"/>
     </row>
     <row r="54" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E54" s="27"/>
-      <c r="F54" s="27"/>
-      <c r="G54" s="31"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="9"/>
     </row>
     <row r="55" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E55" s="27"/>
-      <c r="F55" s="27"/>
-      <c r="G55" s="31"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="9"/>
     </row>
     <row r="56" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E56" s="27"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="31"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="9"/>
     </row>
     <row r="57" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E57" s="27"/>
-      <c r="G57" s="32"/>
+      <c r="E57" s="5"/>
+      <c r="G57" s="10"/>
     </row>
     <row r="58" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E58" s="30"/>
+      <c r="E58" s="26"/>
     </row>
     <row r="59" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E59" s="27"/>
-      <c r="F59" s="27"/>
-      <c r="G59" s="31"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="9"/>
     </row>
     <row r="60" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E60" s="27"/>
-      <c r="F60" s="27"/>
-      <c r="G60" s="31"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="9"/>
     </row>
     <row r="61" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E61" s="27"/>
-      <c r="F61" s="27"/>
-      <c r="G61" s="31"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="9"/>
     </row>
     <row r="62" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E62" s="27"/>
-      <c r="F62" s="27"/>
-      <c r="G62" s="31"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="9"/>
     </row>
     <row r="66" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E66" s="26"/>
+      <c r="E66" s="23"/>
     </row>
     <row r="71" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="F71" s="33"/>
-      <c r="G71" s="33"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
     </row>
     <row r="72" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="F72" s="33"/>
-      <c r="G72" s="33"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
     </row>
     <row r="73" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="F73" s="33"/>
-      <c r="G73" s="33"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
     </row>
     <row r="74" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E74" s="30"/>
+      <c r="E74" s="26"/>
     </row>
     <row r="75" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E75" s="27"/>
+      <c r="E75" s="5"/>
     </row>
     <row r="76" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E76" s="27"/>
-      <c r="F76" s="33"/>
-      <c r="G76" s="33"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
     </row>
     <row r="77" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E77" s="27"/>
+      <c r="E77" s="5"/>
     </row>
     <row r="78" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E78" s="26"/>
-      <c r="F78" s="34"/>
-      <c r="G78" s="34"/>
+      <c r="E78" s="23"/>
+      <c r="F78" s="27"/>
+      <c r="G78" s="27"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J2:L89">

</xml_diff>

<commit_message>
Adding Time Since Fire Effect size plots
</commit_message>
<xml_diff>
--- a/FireMeta_Rproj/inputs/Studies_Summary/Fire_name_Lat_Long.xlsx
+++ b/FireMeta_Rproj/inputs/Studies_Summary/Fire_name_Lat_Long.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cava304/GitHub/rc_sfa-rc-3-wenas-meta/FireMeta_Rproj/inputs/Studies_Summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0727CC39-C012-5444-B327-0FEB1B79F189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBE0E33-C90E-744E-A7F6-97A777AC5850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49640" yWindow="0" windowWidth="19000" windowHeight="24000" xr2:uid="{8C258C6F-044A-E849-9C14-F26FA5F5AA92}"/>
+    <workbookView xWindow="30240" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{8C258C6F-044A-E849-9C14-F26FA5F5AA92}"/>
   </bookViews>
   <sheets>
     <sheet name="Temporal Normalization Studies" sheetId="1" r:id="rId1"/>
@@ -447,9 +447,6 @@
   </si>
   <si>
     <t>Y_not quite the same watershed, and the sus points doesn’t get the exact one correctly</t>
-  </si>
-  <si>
-    <t>Y_pretty far off, looks like it is a subset of the Benjamin slough COMID</t>
   </si>
   <si>
     <t>Y_pretty far off, the sus points doesn’t get the correct watershed</t>
@@ -836,6 +833,9 @@
   </si>
   <si>
     <t>Writer &amp; Murphy, 2012</t>
+  </si>
+  <si>
+    <t>Y_pretty far off, looks like it is a subset of the Benjamin slough COMID, Had to change the comid and now we are good</t>
   </si>
 </sst>
 </file>
@@ -995,7 +995,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1026,9 +1026,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1373,8 +1371,8 @@
   <dimension ref="A1:L178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C178" sqref="C178"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1733,7 +1731,7 @@
         <v>98</v>
       </c>
       <c r="L13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -1853,7 +1851,7 @@
         <v>98</v>
       </c>
       <c r="L17" t="s">
-        <v>129</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1913,7 +1911,7 @@
         <v>98</v>
       </c>
       <c r="L19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -2516,7 +2514,7 @@
       </c>
       <c r="C42" s="10"/>
       <c r="D42" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E42" s="15"/>
       <c r="F42" s="15"/>
@@ -3484,7 +3482,7 @@
       </c>
       <c r="C78" s="10"/>
       <c r="D78" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
@@ -3576,240 +3574,240 @@
     </row>
     <row r="82" spans="2:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B82" s="28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="83" spans="2:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B83" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D83" s="29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C84" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="85" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C85" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="86" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C86" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="87" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C87" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C88" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="89" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C89" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="90" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C90" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="91" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C91" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="92" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C92" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="93" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C93" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="94" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C94" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="95" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C95" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="96" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C96" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C97" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C98" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C99" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C100" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C101" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="102" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C102" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="103" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C103" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="104" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C104" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="105" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C105" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="106" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C106" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="107" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C107" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="108" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C108" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="109" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C109" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="110" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C110" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="111" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C111" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="112" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C112" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C113" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C114" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C115" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C116" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C117" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C118" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C119" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="120" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C120" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C121" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="122" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C122" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="123" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C123" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="124" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C124" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="125" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C125" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C126" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="127" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C127" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="128" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B128" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D128" s="29" t="s">
         <v>104</v>
@@ -3817,7 +3815,7 @@
     </row>
     <row r="129" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C129" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E129">
         <v>65.156433000000007</v>
@@ -3841,12 +3839,12 @@
         <v>96</v>
       </c>
       <c r="L129" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="130" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C130" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E130">
         <v>65.159576999999999</v>
@@ -3870,12 +3868,12 @@
         <v>96</v>
       </c>
       <c r="L130" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="131" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C131" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E131">
         <v>65.158680000000004</v>
@@ -3899,12 +3897,12 @@
         <v>96</v>
       </c>
       <c r="L131" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="132" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C132" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E132">
         <v>65.180338000000006</v>
@@ -3928,15 +3926,15 @@
         <v>96</v>
       </c>
       <c r="L132" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="133" spans="2:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B133" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D133" s="29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="134" spans="2:12" x14ac:dyDescent="0.2">
@@ -3967,7 +3965,7 @@
     </row>
     <row r="135" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C135" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E135">
         <v>34.482937999999997</v>
@@ -3993,7 +3991,7 @@
     </row>
     <row r="136" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C136" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E136">
         <v>34.506217999999997</v>
@@ -4019,7 +4017,7 @@
     </row>
     <row r="137" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C137" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E137">
         <v>34.458570999999999</v>
@@ -4045,7 +4043,7 @@
     </row>
     <row r="138" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C138" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E138">
         <v>34.492925</v>
@@ -4097,7 +4095,7 @@
     </row>
     <row r="140" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C140" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E140">
         <v>34.452924000000003</v>
@@ -4123,7 +4121,7 @@
     </row>
     <row r="141" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C141" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E141">
         <v>34.456563000000003</v>
@@ -4149,7 +4147,7 @@
     </row>
     <row r="142" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C142" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E142">
         <v>34.443747000000002</v>
@@ -4175,7 +4173,7 @@
     </row>
     <row r="143" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C143" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E143">
         <v>34.464474000000003</v>
@@ -4201,7 +4199,7 @@
     </row>
     <row r="144" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C144" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E144">
         <v>34.470762999999998</v>
@@ -4227,7 +4225,7 @@
     </row>
     <row r="145" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C145" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E145">
         <v>34.465553</v>
@@ -4253,7 +4251,7 @@
     </row>
     <row r="146" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C146" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E146">
         <v>34.460483000000004</v>
@@ -4279,7 +4277,7 @@
     </row>
     <row r="147" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C147" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E147">
         <v>34.467247999999998</v>
@@ -4305,15 +4303,15 @@
     </row>
     <row r="148" spans="2:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B148" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D148" s="29" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="149" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C149" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G149">
         <v>10.59</v>
@@ -4336,7 +4334,7 @@
     </row>
     <row r="150" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C150" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G150">
         <v>8.2899999999999991</v>
@@ -4359,7 +4357,7 @@
     </row>
     <row r="151" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C151" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G151">
         <v>3.59</v>
@@ -4382,7 +4380,7 @@
     </row>
     <row r="152" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C152" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G152">
         <v>8.2100000000000009</v>
@@ -4405,7 +4403,7 @@
     </row>
     <row r="153" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C153" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G153">
         <v>7.13</v>
@@ -4428,7 +4426,7 @@
     </row>
     <row r="154" spans="2:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B154" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D154" s="29" t="s">
         <v>113</v>
@@ -4436,7 +4434,7 @@
     </row>
     <row r="155" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C155" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E155">
         <v>35.173952</v>
@@ -4451,18 +4449,18 @@
         <v>93</v>
       </c>
       <c r="J155" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K155" t="s">
         <v>96</v>
       </c>
       <c r="L155" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="156" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C156" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E156">
         <v>35.167361999999997</v>
@@ -4477,18 +4475,18 @@
         <v>93</v>
       </c>
       <c r="J156" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K156" t="s">
         <v>96</v>
       </c>
       <c r="L156" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="157" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C157" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E157">
         <v>35.183095999999999</v>
@@ -4503,18 +4501,18 @@
         <v>93</v>
       </c>
       <c r="J157" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K157" t="s">
         <v>96</v>
       </c>
       <c r="L157" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="158" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C158" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E158">
         <v>35.175843</v>
@@ -4529,18 +4527,18 @@
         <v>93</v>
       </c>
       <c r="J158" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K158" t="s">
         <v>96</v>
       </c>
       <c r="L158" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="159" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C159" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E159">
         <v>35.260796999999997</v>
@@ -4555,18 +4553,18 @@
         <v>93</v>
       </c>
       <c r="J159" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K159" t="s">
         <v>96</v>
       </c>
       <c r="L159" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="160" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C160" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E160">
         <v>35.278956999999998</v>
@@ -4581,18 +4579,18 @@
         <v>93</v>
       </c>
       <c r="J160" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K160" t="s">
         <v>96</v>
       </c>
       <c r="L160" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="161" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C161" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E161">
         <v>35.268053000000002</v>
@@ -4607,18 +4605,18 @@
         <v>93</v>
       </c>
       <c r="J161" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K161" t="s">
         <v>96</v>
       </c>
       <c r="L161" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="162" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C162" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E162">
         <v>35.271836999999998</v>
@@ -4633,29 +4631,29 @@
         <v>93</v>
       </c>
       <c r="J162" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K162" t="s">
         <v>96</v>
       </c>
       <c r="L162" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="163" spans="2:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B163" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="D163" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="D163" s="17" t="s">
+    </row>
+    <row r="164" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B164" s="4"/>
+      <c r="C164" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="164" spans="2:12" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B164" s="31"/>
-      <c r="C164" t="s">
-        <v>222</v>
-      </c>
-      <c r="D164" s="32"/>
+      <c r="D164" s="30"/>
       <c r="E164">
         <v>35.875900000000001</v>
       </c>
@@ -4665,19 +4663,19 @@
       <c r="G164">
         <v>2.4209999999999998</v>
       </c>
-      <c r="I164" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="J164" s="30" t="s">
-        <v>225</v>
-      </c>
-      <c r="K164" s="30" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="165" spans="2:12" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I164" t="s">
+        <v>93</v>
+      </c>
+      <c r="J164" t="s">
+        <v>224</v>
+      </c>
+      <c r="K164" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="165" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C165" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E165">
         <v>35.866700000000002</v>
@@ -4688,22 +4686,22 @@
       <c r="G165">
         <v>3.6720000000000002</v>
       </c>
-      <c r="I165" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="J165" s="30" t="s">
-        <v>225</v>
-      </c>
-      <c r="K165" s="30" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="166" spans="2:12" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B166" s="31"/>
+      <c r="I165" t="s">
+        <v>93</v>
+      </c>
+      <c r="J165" t="s">
+        <v>224</v>
+      </c>
+      <c r="K165" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="166" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B166" s="4"/>
       <c r="C166" t="s">
-        <v>224</v>
-      </c>
-      <c r="D166" s="32"/>
+        <v>223</v>
+      </c>
+      <c r="D166" s="30"/>
       <c r="E166">
         <v>35.909199999999998</v>
       </c>
@@ -4713,75 +4711,75 @@
       <c r="G166">
         <v>3.0550000000000002</v>
       </c>
-      <c r="I166" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="J166" s="30" t="s">
-        <v>225</v>
-      </c>
-      <c r="K166" s="30" t="s">
+      <c r="I166" t="s">
+        <v>93</v>
+      </c>
+      <c r="J166" t="s">
+        <v>224</v>
+      </c>
+      <c r="K166" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="167" spans="2:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B167" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="D167" s="11" t="s">
         <v>226</v>
-      </c>
-      <c r="D167" s="11" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="168" spans="2:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B168" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D168" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="169" spans="2:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B169" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="D169" s="11" t="s">
         <v>230</v>
-      </c>
-      <c r="D169" s="11" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="170" spans="2:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B170" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D170" s="11" t="s">
         <v>232</v>
-      </c>
-      <c r="D170" s="11" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="171" spans="2:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B171" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="D171" s="11" t="s">
         <v>234</v>
-      </c>
-      <c r="D171" s="11" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="172" spans="2:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B172" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D172" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="173" spans="2:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B173" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D173" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="174" spans="2:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B174" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D174" s="13" t="s">
         <v>18</v>
@@ -4789,12 +4787,12 @@
     </row>
     <row r="175" spans="2:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B175" s="28" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="176" spans="2:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B176" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D176" s="11" t="s">
         <v>106</v>
@@ -4802,7 +4800,7 @@
     </row>
     <row r="177" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B177" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D177" s="11" t="s">
         <v>107</v>
@@ -4810,7 +4808,7 @@
     </row>
     <row r="178" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B178" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D178" s="11" t="s">
         <v>105</v>

</xml_diff>